<commit_message>
new encoding practice trials, lab photo size decreased,cannot proceed without consent
</commit_message>
<xml_diff>
--- a/html/resources/stimuli_tables/stimuli_demo.xlsx
+++ b/html/resources/stimuli_tables/stimuli_demo.xlsx
@@ -149,11 +149,12 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="General"/>
   </numFmts>
-  <fonts count="4">
+  <fonts count="5">
     <font>
       <sz val="10"/>
       <name val="Arial"/>
       <family val="2"/>
+      <charset val="1"/>
     </font>
     <font>
       <sz val="10"/>
@@ -169,6 +170,13 @@
       <sz val="10"/>
       <name val="Arial"/>
       <family val="0"/>
+    </font>
+    <font>
+      <b val="true"/>
+      <sz val="10"/>
+      <name val="Arial"/>
+      <family val="2"/>
+      <charset val="1"/>
     </font>
   </fonts>
   <fills count="2">
@@ -213,8 +221,12 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="2">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -238,7 +250,7 @@
   <dimension ref="A1:L11"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
+      <selection pane="topLeft" activeCell="D7" activeCellId="0" sqref="D7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -379,7 +391,7 @@
       <c r="C4" s="0" t="s">
         <v>14</v>
       </c>
-      <c r="D4" s="0" t="s">
+      <c r="D4" s="1" t="s">
         <v>21</v>
       </c>
       <c r="E4" s="0" t="s">
@@ -417,7 +429,7 @@
       <c r="C5" s="0" t="s">
         <v>14</v>
       </c>
-      <c r="D5" s="0" t="s">
+      <c r="D5" s="1" t="s">
         <v>23</v>
       </c>
       <c r="E5" s="0" t="s">
@@ -493,7 +505,7 @@
       <c r="C7" s="0" t="s">
         <v>14</v>
       </c>
-      <c r="D7" s="0" t="s">
+      <c r="D7" s="1" t="s">
         <v>31</v>
       </c>
       <c r="E7" s="0" t="s">
@@ -531,7 +543,7 @@
       <c r="C8" s="0" t="s">
         <v>14</v>
       </c>
-      <c r="D8" s="0" t="s">
+      <c r="D8" s="1" t="s">
         <v>34</v>
       </c>
       <c r="E8" s="0" t="s">
@@ -569,7 +581,7 @@
       <c r="C9" s="0" t="s">
         <v>14</v>
       </c>
-      <c r="D9" s="0" t="s">
+      <c r="D9" s="1" t="s">
         <v>36</v>
       </c>
       <c r="E9" s="0" t="s">
@@ -607,7 +619,7 @@
       <c r="C10" s="0" t="s">
         <v>26</v>
       </c>
-      <c r="D10" s="0" t="s">
+      <c r="D10" s="1" t="s">
         <v>21</v>
       </c>
       <c r="E10" s="0" t="s">
@@ -645,7 +657,7 @@
       <c r="C11" s="0" t="s">
         <v>26</v>
       </c>
-      <c r="D11" s="0" t="s">
+      <c r="D11" s="1" t="s">
         <v>21</v>
       </c>
       <c r="E11" s="0" t="s">

</xml_diff>